<commit_message>
Download Items for Bulk Operations
</commit_message>
<xml_diff>
--- a/LinoVative.Web.Api/Resources/ExcelFiles/UpdateCategoryTemplate.xlsx
+++ b/LinoVative.Web.Api/Resources/ExcelFiles/UpdateCategoryTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\LinoValtiveSolutions\LinoVative.Web.Api\Resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED4B266-9B8D-4E39-A4C5-47D1BD0E8636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243798CE-F715-426D-A079-6D2B0514EDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDEE30A6-2B18-41C6-85EB-1999D5C66F47}"/>
   </bookViews>
@@ -34,19 +34,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Item Category Name</t>
+    <t>ID</t>
   </si>
   <si>
-    <t>Item Group Name</t>
+    <t>Group Name</t>
+  </si>
+  <si>
+    <t>Category Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +58,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="2" tint="-0.749992370372631"/>
       <name val="Aptos Narrow"/>
@@ -88,9 +100,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,21 +438,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56733355-42C7-4069-9CC5-8A34B990EF30}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>